<commit_message>
Committing the latest config file
</commit_message>
<xml_diff>
--- a/simulations/monteCarlo/config.xlsx
+++ b/simulations/monteCarlo/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Repositories\rocket2020\simulations\monteCarlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAC7483-67E4-4F18-AFAA-2CF7218FBF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FBE9A5-999C-4EF5-A72C-10CA3B7FF15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="2595" windowWidth="21600" windowHeight="11385" tabRatio="894" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="2745" windowWidth="21600" windowHeight="11385" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="224">
   <si>
     <t>Value</t>
   </si>
@@ -155,9 +155,6 @@
     <t>sig_gyroz</t>
   </si>
   <si>
-    <t>flightSimFilename</t>
-  </si>
-  <si>
     <t>3-sigma steady-state accel bias</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>m/s/sqrt(hr)</t>
   </si>
   <si>
-    <t>flightData.txt</t>
-  </si>
-  <si>
     <t>injectErrorEnable</t>
   </si>
   <si>
@@ -254,153 +248,9 @@
     <t>m^3/s^2</t>
   </si>
   <si>
-    <t>sig_rbx</t>
-  </si>
-  <si>
-    <t>sig_rby</t>
-  </si>
-  <si>
-    <t>sig_rbz</t>
-  </si>
-  <si>
-    <t>sig_rsx</t>
-  </si>
-  <si>
-    <t>sig_rsy</t>
-  </si>
-  <si>
-    <t>sig_rsz</t>
-  </si>
-  <si>
-    <t>sig_vsx</t>
-  </si>
-  <si>
-    <t>sig_vsy</t>
-  </si>
-  <si>
-    <t>sig_vsz</t>
-  </si>
-  <si>
-    <t>sig_gravx</t>
-  </si>
-  <si>
-    <t>sig_gravy</t>
-  </si>
-  <si>
-    <t>sig_gravz</t>
-  </si>
-  <si>
-    <t>sig_thscx</t>
-  </si>
-  <si>
-    <t>sig_thscy</t>
-  </si>
-  <si>
-    <t>sig_thscz</t>
-  </si>
-  <si>
-    <t>sig_thtcz</t>
-  </si>
-  <si>
-    <t>sig_thtcy</t>
-  </si>
-  <si>
-    <t>sig_thtcx</t>
-  </si>
-  <si>
-    <t>3-sigma initial beacon position uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial satellite position uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial satellite velocity uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial satellite orientation uncertainty</t>
-  </si>
-  <si>
-    <t>sig_range</t>
-  </si>
-  <si>
-    <t>3-sigma initial range bias uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial dopler bias uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial star camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma initial terrain camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t>sig_rfx</t>
-  </si>
-  <si>
-    <t>sig_rfy</t>
-  </si>
-  <si>
-    <t>sig_rfz</t>
-  </si>
-  <si>
-    <t>3-sigma initial feature position uncertainty</t>
-  </si>
-  <si>
-    <t>r_bx</t>
-  </si>
-  <si>
-    <t>r_by</t>
-  </si>
-  <si>
-    <t>r_bz</t>
-  </si>
-  <si>
-    <t>Beacon initial lunar fixed position</t>
-  </si>
-  <si>
-    <t>a_s</t>
-  </si>
-  <si>
-    <t>e_s</t>
-  </si>
-  <si>
-    <t>i_s</t>
-  </si>
-  <si>
-    <t>W_s</t>
-  </si>
-  <si>
-    <t>nu_s</t>
-  </si>
-  <si>
-    <t>w_s</t>
-  </si>
-  <si>
-    <t>Satellite initial orbit semi-major axis</t>
-  </si>
-  <si>
-    <t>Satellite initial orbit eccentricity</t>
-  </si>
-  <si>
-    <t>Satellite initial orbit inclination</t>
-  </si>
-  <si>
     <t>degrees</t>
   </si>
   <si>
-    <t>r_fx</t>
-  </si>
-  <si>
-    <t>r_fy</t>
-  </si>
-  <si>
-    <t>r_fz</t>
-  </si>
-  <si>
-    <t>Feature initial lunar fixed position</t>
-  </si>
-  <si>
     <t>dt</t>
   </si>
   <si>
@@ -413,75 +263,12 @@
     <t>Simulation time</t>
   </si>
   <si>
-    <t>sig_doppler</t>
-  </si>
-  <si>
-    <t>Satellite initial orbit RAAN</t>
-  </si>
-  <si>
-    <t>Satellite initial orbit argument of perigee</t>
-  </si>
-  <si>
-    <t>Satellite initial true anomaly</t>
-  </si>
-  <si>
     <t>measPertCheckEnable</t>
   </si>
   <si>
     <t>flag to enable measurement perturbation check</t>
   </si>
   <si>
-    <t>sig_range_ss</t>
-  </si>
-  <si>
-    <t>3-sigma steady-state range bias</t>
-  </si>
-  <si>
-    <t>sig_doppler_ss</t>
-  </si>
-  <si>
-    <t>3-sigma steady-state doppler bias</t>
-  </si>
-  <si>
-    <t>sig_sc_ss</t>
-  </si>
-  <si>
-    <t>3-sigma steady-state star camera misalignment</t>
-  </si>
-  <si>
-    <t>sig_tc_ss</t>
-  </si>
-  <si>
-    <t>3-sigma steady-state terrain camera misalignment</t>
-  </si>
-  <si>
-    <t>sig_grav_ss</t>
-  </si>
-  <si>
-    <t>3-sigma steady-state gravity bias</t>
-  </si>
-  <si>
-    <t>sig_meas_range</t>
-  </si>
-  <si>
-    <t>sig_meas_doppler</t>
-  </si>
-  <si>
-    <t>sig_meas_scx</t>
-  </si>
-  <si>
-    <t>sig_meas_scy</t>
-  </si>
-  <si>
-    <t>sig_meas_scz</t>
-  </si>
-  <si>
-    <t>sig_meas_tcx</t>
-  </si>
-  <si>
-    <t>sig_meas_tcy</t>
-  </si>
-  <si>
     <t>3-sigma range measurement uncertainty</t>
   </si>
   <si>
@@ -491,15 +278,6 @@
     <t>m/s</t>
   </si>
   <si>
-    <t>3-sigma star camera measurement uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma terrain camera x measurement uncertainty</t>
-  </si>
-  <si>
-    <t>3-sigma terrain camera y measurement uncertainty</t>
-  </si>
-  <si>
     <t>Q_a</t>
   </si>
   <si>
@@ -515,9 +293,6 @@
     <t>arcsec</t>
   </si>
   <si>
-    <t>arcsec/axis</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -527,9 +302,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>3-sigma initial grav bias uncertainty</t>
-  </si>
-  <si>
     <t>del_rx</t>
   </si>
   <si>
@@ -605,9 +377,6 @@
     <t>tau_wind</t>
   </si>
   <si>
-    <t>flight simulation filename (Not used)</t>
-  </si>
-  <si>
     <t>R_E</t>
   </si>
   <si>
@@ -653,15 +422,9 @@
     <t>l_ref</t>
   </si>
   <si>
-    <t>motor</t>
-  </si>
-  <si>
     <t>A_e</t>
   </si>
   <si>
-    <t>commercial</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -692,9 +455,6 @@
     <t>Specific impulse</t>
   </si>
   <si>
-    <t>motor type</t>
-  </si>
-  <si>
     <t>nozzle exit area</t>
   </si>
   <si>
@@ -794,9 +554,6 @@
     <t>Mass moment of inertia about yz</t>
   </si>
   <si>
-    <t>C_L</t>
-  </si>
-  <si>
     <t>C_D</t>
   </si>
   <si>
@@ -822,6 +579,144 @@
   </si>
   <si>
     <t>m_total</t>
+  </si>
+  <si>
+    <t>sig_alt_ss</t>
+  </si>
+  <si>
+    <t>sig_air_ss</t>
+  </si>
+  <si>
+    <t>sig_meas_alt</t>
+  </si>
+  <si>
+    <t>sig_meas_air</t>
+  </si>
+  <si>
+    <t>sig_wind_ss</t>
+  </si>
+  <si>
+    <t>sig_rx</t>
+  </si>
+  <si>
+    <t>sig_ry</t>
+  </si>
+  <si>
+    <t>sig_rz</t>
+  </si>
+  <si>
+    <t>sig_vx</t>
+  </si>
+  <si>
+    <t>sig_vy</t>
+  </si>
+  <si>
+    <t>sig_vz</t>
+  </si>
+  <si>
+    <t>sig_accelx</t>
+  </si>
+  <si>
+    <t>sig_accely</t>
+  </si>
+  <si>
+    <t>sig_accelz</t>
+  </si>
+  <si>
+    <t>sig_alt</t>
+  </si>
+  <si>
+    <t>sig_air</t>
+  </si>
+  <si>
+    <t>sig_wind</t>
+  </si>
+  <si>
+    <t>3-sigma initial accelerometer bias uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma steady-state altimeter bias</t>
+  </si>
+  <si>
+    <t>3-sigma steady-state airspeed bias</t>
+  </si>
+  <si>
+    <t>3-sigma steady-state windspeed</t>
+  </si>
+  <si>
+    <t>3-sigma initial position uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma initial velocity uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma initial attitude uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma initial altimeter bias uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma initial airspeed bias uncertainty</t>
+  </si>
+  <si>
+    <t>3-sigma initial windspeed uncertainty</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>Initial latitude</t>
+  </si>
+  <si>
+    <t>Initial longitude</t>
+  </si>
+  <si>
+    <t>Initial altitude</t>
+  </si>
+  <si>
+    <t>azimuth</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>tail_d</t>
+  </si>
+  <si>
+    <t>tail_D</t>
+  </si>
+  <si>
+    <t>Launch rail azimuth</t>
+  </si>
+  <si>
+    <t>Launch rail elevation</t>
+  </si>
+  <si>
+    <t>l_rail</t>
+  </si>
+  <si>
+    <t>Launch rail length</t>
+  </si>
+  <si>
+    <t>C_L_alpha</t>
+  </si>
+  <si>
+    <t>C_L_0</t>
+  </si>
+  <si>
+    <t>C_L_beta</t>
+  </si>
+  <si>
+    <t>deg^-1</t>
   </si>
 </sst>
 </file>
@@ -834,7 +729,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.000E+00"/>
-    <numFmt numFmtId="179" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1005,13 +900,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1350,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1403,44 +1298,43 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="B3" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B4" s="12">
-        <f>60*2</f>
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="26">
         <v>25</v>
@@ -1521,10 +1415,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="19">
-        <f t="shared" ref="E9:E14" si="1">B9</f>
+        <f t="shared" ref="E9:E13" si="1">B9</f>
         <v>3500</v>
       </c>
     </row>
@@ -1539,7 +1433,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="19">
         <f t="shared" si="1"/>
@@ -1548,7 +1442,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="B11" s="15">
         <v>3500</v>
@@ -1557,7 +1451,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="1"/>
@@ -1566,7 +1460,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>184</v>
+        <v>108</v>
       </c>
       <c r="B12" s="15">
         <v>3500</v>
@@ -1575,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="1"/>
@@ -1584,7 +1478,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>185</v>
+        <v>109</v>
       </c>
       <c r="B13" s="15">
         <v>2000</v>
@@ -1593,7 +1487,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="1"/>
@@ -1601,26 +1495,26 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>47</v>
+      <c r="A14" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14" s="19" t="str">
-        <f t="shared" si="1"/>
-        <v>flightData.txt</v>
+        <v>47</v>
+      </c>
+      <c r="E14" s="19">
+        <f>B14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B15" s="12">
         <v>0</v>
@@ -1629,7 +1523,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E15" s="19">
         <f>B15</f>
@@ -1637,38 +1531,20 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="12">
+      <c r="A16" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="27">
         <v>0</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="19">
+      <c r="D16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="21">
         <f>B16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="27">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" s="21">
-        <f>B17</f>
         <v>0</v>
       </c>
     </row>
@@ -1693,7 +1569,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1">
         <v>60</v>
@@ -1701,7 +1577,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>60</v>
@@ -1709,7 +1585,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <f>hr2min*min2sec</f>
@@ -1718,7 +1594,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>9.81</v>
@@ -1734,7 +1610,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,91 +1636,91 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="47">
-        <v>4902801076000</v>
+        <v>63</v>
+      </c>
+      <c r="B2" s="46">
+        <v>399000000000000</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="E2" s="19">
         <f t="shared" ref="E2:E5" si="0">B2</f>
-        <v>4902801076000</v>
+        <v>399000000000000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="48">
-        <v>2.0335424821116E-4</v>
+        <v>64</v>
+      </c>
+      <c r="B3" s="47">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="28" t="s">
-        <v>189</v>
+        <v>112</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
-        <v>2.0335424821116E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="48">
-        <v>1737400</v>
+        <v>110</v>
+      </c>
+      <c r="B4" s="47">
+        <v>6371000</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
-        <v>1737400</v>
+        <v>6371000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="48">
-        <v>1737400</v>
+        <v>65</v>
+      </c>
+      <c r="B5" s="47">
+        <v>6378137</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
-        <v>1737400</v>
+        <v>6378137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B6" s="48">
+        <v>111</v>
+      </c>
+      <c r="B6" s="47">
         <v>9.81</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>193</v>
+        <v>116</v>
       </c>
       <c r="E6" s="19">
         <f>B6</f>
@@ -1859,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2D875C-EDA0-4EF7-BA1F-DC0B7E7A3584}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,26 +1765,25 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="B2" s="39">
-        <f>1737400+10000</f>
-        <v>1747400</v>
+        <v>41.666200000000003</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>110</v>
+        <v>209</v>
       </c>
       <c r="E2" s="18">
-        <f>B2</f>
-        <v>1747400</v>
+        <f>RADIANS(B2)</f>
+        <v>0.72721237679446138</v>
       </c>
       <c r="F2" s="39">
         <v>1767400</v>
@@ -1916,20 +1791,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="26">
-        <v>0</v>
+        <v>206</v>
+      </c>
+      <c r="B3" s="47">
+        <v>-111.4632</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="19">
-        <f>B3</f>
-        <v>0</v>
+        <v>210</v>
+      </c>
+      <c r="E3" s="18">
+        <f>RADIANS(B3)</f>
+        <v>-1.9453998348089436</v>
       </c>
       <c r="F3" s="26">
         <v>0</v>
@@ -1937,20 +1812,20 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="B4" s="12">
-        <v>90</v>
+        <v>1380</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>211</v>
       </c>
       <c r="E4" s="19">
-        <f>RADIANS(B4)</f>
-        <v>1.5707963267948966</v>
+        <f>B4</f>
+        <v>1380</v>
       </c>
       <c r="F4" s="12">
         <v>95</v>
@@ -1958,191 +1833,63 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="26">
-        <v>180</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>113</v>
+        <v>218</v>
+      </c>
+      <c r="B5" s="47">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="E5" s="19">
-        <f>RADIANS(B5)</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="F5" s="26">
-        <v>0</v>
-      </c>
+        <f>B5</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>109</v>
+        <v>212</v>
       </c>
       <c r="B6" s="26">
         <v>90</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="E6" s="19">
         <f>RADIANS(B6)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="F6" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="50">
+        <v>85</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="21">
+        <f>RADIANS(B7)</f>
+        <v>1.4835298641951802</v>
+      </c>
+      <c r="F7" s="26">
         <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="26">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="19">
-        <f>RADIANS(B7)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="15">
-        <v>1737400</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="19">
-        <f t="shared" ref="E8:E13" si="0">B8</f>
-        <v>1737400</v>
-      </c>
-      <c r="F8" s="15">
-        <v>1737400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="12">
-        <v>0</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="20">
-        <v>-1737400</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="21">
-        <f t="shared" si="0"/>
-        <v>-1737400</v>
-      </c>
-      <c r="F13" s="20">
-        <v>1737400</v>
       </c>
     </row>
   </sheetData>
@@ -2153,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B51D10-E8C4-4315-87FD-BE14F62A3085}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,41 +1929,41 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="47">
+        <v>117</v>
+      </c>
+      <c r="B2" s="46">
         <f>PI()*(B4/2)^2</f>
         <v>2.8352873698647883E-2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>206</v>
+        <v>127</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="E2" s="19">
-        <f t="shared" ref="E2:E36" si="0">B2</f>
+        <f t="shared" ref="E2:E40" si="0">B2</f>
         <v>2.8352873698647883E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" s="47">
+        <v>150</v>
+      </c>
+      <c r="B3" s="46">
         <f>PI()*B4*B5</f>
         <v>1.1341149479459152</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>206</v>
+        <v>127</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>231</v>
+        <v>151</v>
       </c>
       <c r="E3" s="19">
         <f>B3</f>
@@ -2225,16 +1972,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="48">
+        <v>118</v>
+      </c>
+      <c r="B4" s="47">
         <v>0.19</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>208</v>
+        <v>129</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
@@ -2243,16 +1990,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="48">
+        <v>124</v>
+      </c>
+      <c r="B5" s="47">
         <v>1.9</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>209</v>
+        <v>130</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
@@ -2261,121 +2008,120 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B6" s="48">
-        <v>0</v>
+        <v>119</v>
+      </c>
+      <c r="B6" s="47">
+        <v>1.98</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>211</v>
+        <v>132</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="48">
-        <v>0</v>
+        <v>120</v>
+      </c>
+      <c r="B7" s="47">
+        <v>1.66</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="48">
-        <v>0</v>
+        <v>121</v>
+      </c>
+      <c r="B8" s="47">
+        <v>1.5</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="B9" s="40">
-        <v>2100</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="A9" s="6" t="s">
         <v>213</v>
       </c>
+      <c r="B9" s="47">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="19">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>200</v>
+        <v>122</v>
       </c>
       <c r="B10" s="40">
-        <v>199</v>
+        <v>2100</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="E10" s="19">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" t="s">
-        <v>204</v>
+        <v>123</v>
+      </c>
+      <c r="B11" s="40">
+        <v>199</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>5</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="E11" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>commercial</v>
+        <v>135</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="0"/>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>203</v>
+        <v>125</v>
       </c>
       <c r="B12" s="40">
         <v>6.1359000000000001E-4</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>127</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>216</v>
+        <v>136</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -2384,7 +2130,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>232</v>
+        <v>152</v>
       </c>
       <c r="B13" s="40">
         <v>0.25</v>
@@ -2393,7 +2139,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>233</v>
+        <v>153</v>
       </c>
       <c r="E13" s="19">
         <f>B13</f>
@@ -2402,17 +2148,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" s="51">
+        <v>143</v>
+      </c>
+      <c r="B14" s="48">
         <f>B13*B15 - 0.5*B15^2*(TAN(E18) + TAN(E19))</f>
         <v>6.7469582591336119E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>127</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>217</v>
+        <v>137</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
@@ -2421,7 +2167,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>224</v>
+        <v>144</v>
       </c>
       <c r="B15" s="40">
         <v>0.3</v>
@@ -2430,7 +2176,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>218</v>
+        <v>138</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="0"/>
@@ -2439,7 +2185,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="B16" s="40">
         <v>0.01</v>
@@ -2448,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="0"/>
@@ -2457,14 +2203,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>226</v>
+        <v>146</v>
       </c>
       <c r="B17" s="2">
         <f>B15^2/B14</f>
         <v>1.3339344419118586</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="E17" s="19">
         <f t="shared" si="0"/>
@@ -2473,16 +2219,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>227</v>
+        <v>147</v>
       </c>
       <c r="B18" s="40">
         <v>9.5</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>149</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>235</v>
+        <v>155</v>
       </c>
       <c r="E18" s="19">
         <f>RADIANS(B18)</f>
@@ -2491,16 +2237,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>234</v>
+        <v>154</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>149</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
       <c r="E19" s="19">
         <f>RADIANS(B19)</f>
@@ -2509,103 +2255,107 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B20" s="40">
-        <v>4</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>221</v>
-      </c>
+        <f>B4</f>
+        <v>0.19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="28"/>
       <c r="E20" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>B20</f>
+        <v>0.19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="B21" s="40">
-        <v>20</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>243</v>
-      </c>
+        <f>B4</f>
+        <v>0.19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="19">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>B21</f>
+        <v>0.19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>238</v>
+        <v>148</v>
       </c>
       <c r="B22" s="40">
-        <v>506</v>
+        <v>4</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>244</v>
+        <v>141</v>
       </c>
       <c r="E22" s="19">
         <f t="shared" si="0"/>
-        <v>506</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="B23" s="40">
-        <v>506</v>
+        <v>20</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>245</v>
+        <v>163</v>
       </c>
       <c r="E23" s="19">
         <f t="shared" si="0"/>
-        <v>506</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="B24" s="40">
-        <v>0</v>
+        <v>506</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>246</v>
+        <v>164</v>
       </c>
       <c r="E24" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>506</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="B25" s="40">
-        <v>15</v>
+        <v>506</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>247</v>
+        <v>165</v>
       </c>
       <c r="E25" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>506</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>242</v>
+        <v>160</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>248</v>
+        <v>166</v>
       </c>
       <c r="E26" s="19">
         <f t="shared" si="0"/>
@@ -2614,155 +2364,209 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>172</v>
+        <v>161</v>
+      </c>
+      <c r="B27" s="40">
+        <v>15</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>167</v>
       </c>
       <c r="E27" s="19">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="B28" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="B28" s="40">
+        <v>0</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="E28" s="19">
         <f t="shared" si="0"/>
-        <v>2E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>172</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B29" s="40">
+        <v>0</v>
+      </c>
+      <c r="D29" s="28"/>
       <c r="E29" s="19">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="B30" s="2">
-        <v>0.4</v>
+        <v>1E-3</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="E30" s="19">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
+        <f>1/RADIANS(1/B30)</f>
+        <v>5.7295779513082318E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="B31" s="2">
-        <v>3.835</v>
+        <v>1E-3</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="E31" s="19">
-        <f t="shared" si="0"/>
-        <v>3.835</v>
+        <f>1/RADIANS(1/B31)</f>
+        <v>5.7295779513082318E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
       <c r="B32" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="E32" s="19">
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E33" s="19">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E34" s="19">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.835</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="19">
+        <f t="shared" si="0"/>
+        <v>3.835</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="2">
         <v>2.4889999999999999</v>
       </c>
-      <c r="C32" t="s">
-        <v>172</v>
-      </c>
-      <c r="E32" s="19">
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="19">
         <f t="shared" si="0"/>
         <v>2.4889999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="B33" s="2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37" s="2">
         <f>1.012+0.984+0.0642</f>
         <v>2.0602</v>
       </c>
-      <c r="C33" t="s">
-        <v>172</v>
-      </c>
-      <c r="E33" s="19">
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="19">
         <f t="shared" si="0"/>
         <v>2.0602</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="B34" s="2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="2">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="C34" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="19">
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="19">
         <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="B35" s="2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="2">
         <v>0.2</v>
       </c>
-      <c r="C35" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="19">
+      <c r="C39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="19">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="B36" s="2">
-        <f>SUM(B27:B35)</f>
-        <v>9.5421999999999993</v>
-      </c>
-      <c r="C36" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="19">
-        <f t="shared" si="0"/>
-        <v>9.5421999999999993</v>
-      </c>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="2">
+        <f>SUM(B30:B39)</f>
+        <v>9.344199999999999</v>
+      </c>
+      <c r="C40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="19">
+        <f t="shared" si="0"/>
+        <v>9.344199999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2772,10 +2576,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,30 +2605,30 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>159</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="B2" s="10">
         <v>1E-10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="E2" s="18">
         <f>B2</f>
@@ -2842,7 +2646,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="19">
         <f>B3*g2mps2/3</f>
@@ -2863,10 +2667,10 @@
         <v>0.6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="21">
         <f>B4/SQRT(hr2sec)/3</f>
@@ -2881,14 +2685,14 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="B5" s="11">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="28" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="E5" s="19">
         <f>B5</f>
@@ -2900,7 +2704,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>10</v>
@@ -2910,7 +2714,7 @@
       </c>
       <c r="E6" s="19">
         <f>RADIANS(B6)/hr2sec/3</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -2927,7 +2731,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="20">
-        <v>0.7</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>14</v>
@@ -2937,7 +2741,7 @@
       </c>
       <c r="E7" s="21">
         <f>RADIANS(B7)/SQRT(hr2sec)/3</f>
-        <v>6.7873915355335033E-5</v>
+        <v>6.7873915355335045E-6</v>
       </c>
       <c r="F7">
         <v>0.7</v>
@@ -2951,7 +2755,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="B8" s="15">
         <v>31.5</v>
@@ -2960,314 +2764,100 @@
         <v>8</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="E8" s="19">
-        <f t="shared" ref="E8:E19" si="0">B8/3</f>
+        <f t="shared" ref="E8:E12" si="0">B8/3</f>
         <v>10.5</v>
-      </c>
-      <c r="F8">
-        <v>31.5</v>
-      </c>
-      <c r="G8">
-        <v>3.15</v>
-      </c>
-      <c r="H8">
-        <v>0.315</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="E9" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>0.3</v>
-      </c>
-      <c r="H9">
-        <v>0.03</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="B10" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="E10" s="19">
-        <f>B10*g2mps2/3</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="46">
-        <v>1.5E-5</v>
-      </c>
+        <f>B10/3</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="15">
-        <v>200</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" s="19">
-        <f>RADIANS(B11)/3600/3</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="F11">
-        <v>200</v>
-      </c>
-      <c r="G11">
-        <v>20</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="15">
-        <v>200</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="19">
-        <f>RADIANS(B12)/3600/3</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="F12">
-        <v>200</v>
-      </c>
-      <c r="G12">
-        <v>20</v>
-      </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="17">
+      <c r="A11" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="17">
         <f>B8</f>
         <v>31.5</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="E13" s="18">
+      <c r="D11" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="18">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
-      <c r="F13">
-        <v>31.5</v>
-      </c>
-      <c r="G13">
-        <v>3.15</v>
-      </c>
-      <c r="H13">
-        <v>0.315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="15">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="20">
         <f>B9</f>
         <v>3</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="C12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>0.3</v>
-      </c>
-      <c r="H14">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="19">
-        <f>RADIANS(B15)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
-      <c r="F15">
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <v>3.5</v>
-      </c>
-      <c r="H15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="19">
-        <f t="shared" ref="E16:E17" si="1">RADIANS(B16)/3600/3</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
-      <c r="F16">
-        <v>6</v>
-      </c>
-      <c r="G16">
-        <v>3.5</v>
-      </c>
-      <c r="H16">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="15">
-        <v>9</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" s="19">
-        <f t="shared" si="1"/>
-        <v>1.4544410433286079E-5</v>
-      </c>
-      <c r="F17">
-        <v>30</v>
-      </c>
-      <c r="G17">
-        <v>21</v>
-      </c>
-      <c r="H17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="15">
-        <f>RADIANS(40)/1920*10</f>
-        <v>3.6361026083215199E-3</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E18" s="19">
-        <f t="shared" si="0"/>
-        <v>1.2120342027738399E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B19" s="20">
-        <f>RADIANS(40)/1920*10</f>
-        <v>3.6361026083215199E-3</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="21">
-        <f t="shared" si="0"/>
-        <v>1.2120342027738399E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E10" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,12 +2885,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="B2" s="5">
         <v>500</v>
@@ -3309,28 +2899,19 @@
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="E2" s="18">
         <f t="shared" ref="E2:E13" si="0">B2/3</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="F2" s="7">
-        <v>86</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1500</v>
-      </c>
-      <c r="H2" s="7">
-        <v>10000</v>
-      </c>
       <c r="J2" s="5">
         <v>4500</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="B3" s="7">
         <v>500</v>
@@ -3339,20 +2920,11 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
         <v>166.66666666666666</v>
-      </c>
-      <c r="F3" s="7">
-        <v>70</v>
-      </c>
-      <c r="G3" s="7">
-        <v>200</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1000</v>
       </c>
       <c r="J3" s="7">
         <v>600</v>
@@ -3360,7 +2932,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>74</v>
+        <v>185</v>
       </c>
       <c r="B4" s="7">
         <v>500</v>
@@ -3369,20 +2941,11 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
         <v>166.66666666666666</v>
-      </c>
-      <c r="F4" s="7">
-        <v>10</v>
-      </c>
-      <c r="G4" s="7">
-        <v>50</v>
-      </c>
-      <c r="H4" s="7">
-        <v>300</v>
       </c>
       <c r="J4" s="7">
         <v>150</v>
@@ -3390,7 +2953,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="B5" s="7">
         <v>0.2</v>
@@ -3399,21 +2962,15 @@
         <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F5" s="28">
-        <v>9.4999999999999998E-3</v>
-      </c>
-      <c r="G5" s="28">
-        <v>4.7E-2</v>
-      </c>
-      <c r="H5" s="28">
-        <v>0.28000000000000003</v>
-      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="J5" s="7">
         <f>O5*3</f>
         <v>0</v>
@@ -3421,7 +2978,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>187</v>
       </c>
       <c r="B6" s="7">
         <v>0.2</v>
@@ -3430,21 +2987,15 @@
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F6" s="28">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G6" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="H6" s="28">
-        <v>1</v>
-      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="J6" s="7">
         <f t="shared" ref="J6:J7" si="1">O6*3</f>
         <v>0</v>
@@ -3452,7 +3003,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>77</v>
+        <v>188</v>
       </c>
       <c r="B7" s="7">
         <v>0.2</v>
@@ -3461,21 +3012,15 @@
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F7" s="28">
-        <v>0.08</v>
-      </c>
-      <c r="G7" s="28">
-        <v>1.5</v>
-      </c>
-      <c r="H7" s="28">
-        <v>9.5</v>
-      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
       <c r="J7" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3489,10 +3034,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="E8" s="19">
         <f>RADIANS(B8)/3600/3</f>
@@ -3513,10 +3058,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="E9" s="19">
         <f>RADIANS(B9)/3600/3</f>
@@ -3537,10 +3082,10 @@
         <v>30</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="E10" s="19">
         <f>RADIANS(B10)/3600/3</f>
@@ -3555,7 +3100,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>69</v>
+        <v>189</v>
       </c>
       <c r="B11" s="12">
         <v>5</v>
@@ -3564,7 +3109,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
@@ -3576,7 +3121,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="B12" s="12">
         <v>5</v>
@@ -3585,7 +3130,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -3597,7 +3142,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>191</v>
       </c>
       <c r="B13" s="12">
         <v>10</v>
@@ -3606,7 +3151,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="0"/>
@@ -3622,7 +3167,7 @@
       </c>
       <c r="B14" s="12">
         <f>truthStateParams!B6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14" s="11" t="str">
         <f>truthStateParams!$C$6</f>
@@ -3633,20 +3178,20 @@
       </c>
       <c r="E14" s="19">
         <f>RADIANS(B14)/hr2sec/3</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
       <c r="J14" s="12">
         <f>truthStateParams!$B$6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="47">
         <f>truthStateParams!B6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C15" s="11" t="str">
         <f>truthStateParams!$C$6</f>
@@ -3657,20 +3202,20 @@
       </c>
       <c r="E15" s="19">
         <f>RADIANS(B15)/hr2sec/3</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
       <c r="J15" s="12">
         <f>truthStateParams!$B$6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="47">
         <f>truthStateParams!B6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16" s="11" t="str">
         <f>truthStateParams!$C$6</f>
@@ -3681,16 +3226,16 @@
       </c>
       <c r="E16" s="19">
         <f>RADIANS(B16)/hr2sec/3</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
       <c r="J16" s="12">
         <f>truthStateParams!$B$6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="B17" s="12">
         <f>truthStateParams!B8</f>
@@ -3700,7 +3245,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="E17" s="19">
         <f>B17/3</f>
@@ -3713,7 +3258,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="B18" s="12">
         <f>truthStateParams!B9</f>
@@ -3723,7 +3268,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="E18" s="19">
         <f>B18/3</f>
@@ -3735,278 +3280,27 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="47">
+      <c r="A19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="38">
         <f>truthStateParams!B10</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="25" t="str">
+        <v>5</v>
+      </c>
+      <c r="C19" s="49" t="str">
         <f>truthStateParams!$C$3</f>
         <v>g</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E19" s="19">
+      <c r="D19" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E19" s="21">
         <f>B19*g2mps2/3</f>
-        <v>0</v>
+        <v>16.350000000000001</v>
       </c>
       <c r="J19" s="11">
         <f>truthStateParams!J10</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="47">
-        <f>truthStateParams!B10</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="25" t="str">
-        <f>truthStateParams!$C$3</f>
-        <v>g</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E20" s="19">
-        <f>B20*g2mps2/3</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="J20" s="11">
-        <f>truthStateParams!J10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="47">
-        <f>truthStateParams!B10</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="25" t="str">
-        <f>truthStateParams!$C$3</f>
-        <v>g</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E21" s="19">
-        <f>B21*g2mps2/3</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="11">
-        <f>truthStateParams!J10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="12">
-        <f>truthStateParams!B11</f>
-        <v>200</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="19">
-        <f>RADIANS(B22)/3600/3</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="J22" s="7">
-        <f>truthStateParams!J11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="48">
-        <f>truthStateParams!B11</f>
-        <v>200</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="19">
-        <f t="shared" ref="E23:E27" si="2">RADIANS(B23)/3600/3</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="J23" s="7">
-        <f>truthStateParams!J11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="48">
-        <f>truthStateParams!B11</f>
-        <v>200</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="19">
-        <f t="shared" si="2"/>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="J24" s="7">
-        <f>truthStateParams!J11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="12">
-        <f>truthStateParams!B12</f>
-        <v>200</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="19">
-        <f t="shared" si="2"/>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="J25" s="7">
-        <f>truthStateParams!J12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="48">
-        <f>truthStateParams!B12</f>
-        <v>200</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="19">
-        <f t="shared" si="2"/>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="J26" s="7">
-        <f>truthStateParams!J12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="48">
-        <f>truthStateParams!B12</f>
-        <v>200</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="19">
-        <f t="shared" si="2"/>
-        <v>3.2320912073969063E-4</v>
-      </c>
-      <c r="J27" s="7">
-        <f>truthStateParams!J12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="12">
-        <v>100</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="19">
-        <f t="shared" ref="E28:E30" si="3">B28/3</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="J28" s="28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="12">
-        <v>100</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="19">
-        <f t="shared" si="3"/>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="J29" s="28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="50">
-        <v>100</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="21">
-        <f t="shared" si="3"/>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="J30" s="29">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4017,10 +3311,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4048,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,7 +3443,7 @@
       </c>
       <c r="B6" s="15">
         <f>truthStateParams!B6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C6" s="11" t="str">
         <f>truthStateParams!C6</f>
@@ -4161,7 +3455,7 @@
       </c>
       <c r="E6" s="19">
         <f>truthStateParams!E6</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
       <c r="F6" s="16"/>
     </row>
@@ -4172,7 +3466,7 @@
       </c>
       <c r="B7" s="20">
         <f>truthStateParams!B7</f>
-        <v>0.7</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C7" s="38" t="str">
         <f>truthStateParams!C7</f>
@@ -4184,14 +3478,14 @@
       </c>
       <c r="E7" s="21">
         <f>truthStateParams!E7</f>
-        <v>6.7873915355335033E-5</v>
+        <v>6.7873915355335045E-6</v>
       </c>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>truthStateParams!A8</f>
-        <v>sig_range_ss</v>
+        <v>sig_alt_ss</v>
       </c>
       <c r="B8" s="17">
         <f>truthStateParams!B8</f>
@@ -4203,7 +3497,7 @@
       </c>
       <c r="D8" s="5" t="str">
         <f>truthStateParams!D8</f>
-        <v>3-sigma steady-state range bias</v>
+        <v>3-sigma steady-state altimeter bias</v>
       </c>
       <c r="E8" s="18">
         <f>truthStateParams!E8</f>
@@ -4213,7 +3507,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>truthStateParams!A9</f>
-        <v>sig_doppler_ss</v>
+        <v>sig_air_ss</v>
       </c>
       <c r="B9" s="15">
         <f>truthStateParams!B9</f>
@@ -4225,7 +3519,7 @@
       </c>
       <c r="D9" s="7" t="str">
         <f>truthStateParams!D9</f>
-        <v>3-sigma steady-state doppler bias</v>
+        <v>3-sigma steady-state airspeed bias</v>
       </c>
       <c r="E9" s="19">
         <f>truthStateParams!E9</f>
@@ -4235,221 +3529,67 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>truthStateParams!A10</f>
-        <v>sig_grav_ss</v>
-      </c>
-      <c r="B10" s="47">
+        <v>sig_wind_ss</v>
+      </c>
+      <c r="B10" s="46">
         <f>truthStateParams!B10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="11" t="str">
         <f>truthStateParams!C10</f>
-        <v>g</v>
+        <v>m/s</v>
       </c>
       <c r="D10" s="7" t="str">
         <f>truthStateParams!D10</f>
-        <v>3-sigma steady-state gravity bias</v>
+        <v>3-sigma steady-state windspeed</v>
       </c>
       <c r="E10" s="19">
         <f>truthStateParams!E10</f>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="str">
+      <c r="A11" s="4" t="str">
         <f>truthStateParams!A11</f>
-        <v>sig_sc_ss</v>
-      </c>
-      <c r="B11" s="15">
+        <v>sig_meas_alt</v>
+      </c>
+      <c r="B11" s="17">
         <f>truthStateParams!B11</f>
-        <v>200</v>
-      </c>
-      <c r="C11" s="11" t="str">
+        <v>31.5</v>
+      </c>
+      <c r="C11" s="10" t="str">
         <f>truthStateParams!C11</f>
-        <v>arcsec/axis</v>
-      </c>
-      <c r="D11" s="7" t="str">
+        <v>m</v>
+      </c>
+      <c r="D11" s="5" t="str">
         <f>truthStateParams!D11</f>
-        <v>3-sigma steady-state star camera misalignment</v>
-      </c>
-      <c r="E11" s="19">
+        <v>3-sigma range measurement uncertainty</v>
+      </c>
+      <c r="E11" s="18">
         <f>truthStateParams!E11</f>
-        <v>3.2320912073969063E-4</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>truthStateParams!A12</f>
-        <v>sig_tc_ss</v>
+        <v>sig_meas_air</v>
       </c>
       <c r="B12" s="20">
         <f>truthStateParams!B12</f>
-        <v>200</v>
+        <v>3</v>
       </c>
       <c r="C12" s="38" t="str">
         <f>truthStateParams!C12</f>
-        <v>arcsec/axis</v>
+        <v>m/s</v>
       </c>
       <c r="D12" s="9" t="str">
         <f>truthStateParams!D12</f>
-        <v>3-sigma steady-state terrain camera misalignment</v>
+        <v>3-sigma doppler measurement uncertainty</v>
       </c>
       <c r="E12" s="21">
         <f>truthStateParams!E12</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <f>truthStateParams!A13</f>
-        <v>sig_meas_range</v>
-      </c>
-      <c r="B13" s="17">
-        <f>truthStateParams!B13</f>
-        <v>31.5</v>
-      </c>
-      <c r="C13" s="10" t="str">
-        <f>truthStateParams!C13</f>
-        <v>m</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <f>truthStateParams!D13</f>
-        <v>3-sigma range measurement uncertainty</v>
-      </c>
-      <c r="E13" s="18">
-        <f>truthStateParams!E13</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="str">
-        <f>truthStateParams!A14</f>
-        <v>sig_meas_doppler</v>
-      </c>
-      <c r="B14" s="15">
-        <f>truthStateParams!B14</f>
-        <v>3</v>
-      </c>
-      <c r="C14" s="11" t="str">
-        <f>truthStateParams!C14</f>
-        <v>m/s</v>
-      </c>
-      <c r="D14" s="7" t="str">
-        <f>truthStateParams!D14</f>
-        <v>3-sigma doppler measurement uncertainty</v>
-      </c>
-      <c r="E14" s="19">
-        <f>truthStateParams!E14</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="str">
-        <f>truthStateParams!A15</f>
-        <v>sig_meas_scx</v>
-      </c>
-      <c r="B15" s="15">
-        <f>truthStateParams!B15</f>
-        <v>1.5</v>
-      </c>
-      <c r="C15" s="11" t="str">
-        <f>truthStateParams!C15</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f>truthStateParams!D15</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E15" s="19">
-        <f>truthStateParams!E15</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="str">
-        <f>truthStateParams!A16</f>
-        <v>sig_meas_scy</v>
-      </c>
-      <c r="B16" s="15">
-        <f>truthStateParams!B16</f>
-        <v>1.5</v>
-      </c>
-      <c r="C16" s="11" t="str">
-        <f>truthStateParams!C16</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D16" s="7" t="str">
-        <f>truthStateParams!D16</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E16" s="19">
-        <f>truthStateParams!E16</f>
-        <v>2.4240684055476799E-6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="str">
-        <f>truthStateParams!A17</f>
-        <v>sig_meas_scz</v>
-      </c>
-      <c r="B17" s="15">
-        <f>truthStateParams!B17</f>
-        <v>9</v>
-      </c>
-      <c r="C17" s="11" t="str">
-        <f>truthStateParams!C17</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D17" s="7" t="str">
-        <f>truthStateParams!D17</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E17" s="19">
-        <f>truthStateParams!E17</f>
-        <v>1.4544410433286079E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="str">
-        <f>truthStateParams!A18</f>
-        <v>sig_meas_tcx</v>
-      </c>
-      <c r="B18" s="15">
-        <f>truthStateParams!B18</f>
-        <v>3.6361026083215199E-3</v>
-      </c>
-      <c r="C18" s="11" t="str">
-        <f>truthStateParams!C18</f>
-        <v>rad</v>
-      </c>
-      <c r="D18" s="7" t="str">
-        <f>truthStateParams!D18</f>
-        <v>3-sigma terrain camera x measurement uncertainty</v>
-      </c>
-      <c r="E18" s="19">
-        <f>truthStateParams!E18</f>
-        <v>1.2120342027738399E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="str">
-        <f>truthStateParams!A19</f>
-        <v>sig_meas_tcy</v>
-      </c>
-      <c r="B19" s="20">
-        <f>truthStateParams!B19</f>
-        <v>3.6361026083215199E-3</v>
-      </c>
-      <c r="C19" s="38" t="str">
-        <f>truthStateParams!C19</f>
-        <v>rad</v>
-      </c>
-      <c r="D19" s="9" t="str">
-        <f>truthStateParams!D19</f>
-        <v>3-sigma terrain camera y measurement uncertainty</v>
-      </c>
-      <c r="E19" s="21">
-        <f>truthStateParams!E19</f>
-        <v>1.2120342027738399E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4460,10 +3600,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4490,13 +3630,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>truthStateInitialUncertainty!A2</f>
-        <v>sig_rsx</v>
+        <v>sig_rx</v>
       </c>
       <c r="B2" s="5">
         <f>truthStateInitialUncertainty!B2</f>
@@ -4508,7 +3648,7 @@
       </c>
       <c r="D2" s="5" t="str">
         <f>truthStateInitialUncertainty!D2</f>
-        <v>3-sigma initial satellite position uncertainty</v>
+        <v>3-sigma initial position uncertainty</v>
       </c>
       <c r="E2" s="18">
         <f>truthStateInitialUncertainty!E2</f>
@@ -4518,7 +3658,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>truthStateInitialUncertainty!A3</f>
-        <v>sig_rsy</v>
+        <v>sig_ry</v>
       </c>
       <c r="B3" s="7">
         <f>truthStateInitialUncertainty!B3</f>
@@ -4530,7 +3670,7 @@
       </c>
       <c r="D3" s="7" t="str">
         <f>truthStateInitialUncertainty!D3</f>
-        <v>3-sigma initial satellite position uncertainty</v>
+        <v>3-sigma initial position uncertainty</v>
       </c>
       <c r="E3" s="19">
         <f>truthStateInitialUncertainty!E3</f>
@@ -4540,7 +3680,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>truthStateInitialUncertainty!A4</f>
-        <v>sig_rsz</v>
+        <v>sig_rz</v>
       </c>
       <c r="B4" s="7">
         <f>truthStateInitialUncertainty!B4</f>
@@ -4552,7 +3692,7 @@
       </c>
       <c r="D4" s="7" t="str">
         <f>truthStateInitialUncertainty!D4</f>
-        <v>3-sigma initial satellite position uncertainty</v>
+        <v>3-sigma initial position uncertainty</v>
       </c>
       <c r="E4" s="19">
         <f>truthStateInitialUncertainty!E4</f>
@@ -4562,7 +3702,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>truthStateInitialUncertainty!A5</f>
-        <v>sig_vsx</v>
+        <v>sig_vx</v>
       </c>
       <c r="B5" s="7">
         <f>truthStateInitialUncertainty!B5</f>
@@ -4574,7 +3714,7 @@
       </c>
       <c r="D5" s="7" t="str">
         <f>truthStateInitialUncertainty!D5</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
+        <v>3-sigma initial velocity uncertainty</v>
       </c>
       <c r="E5" s="19">
         <f>truthStateInitialUncertainty!E5</f>
@@ -4584,7 +3724,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>truthStateInitialUncertainty!A6</f>
-        <v>sig_vsy</v>
+        <v>sig_vy</v>
       </c>
       <c r="B6" s="7">
         <f>truthStateInitialUncertainty!B6</f>
@@ -4596,7 +3736,7 @@
       </c>
       <c r="D6" s="7" t="str">
         <f>truthStateInitialUncertainty!D6</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
+        <v>3-sigma initial velocity uncertainty</v>
       </c>
       <c r="E6" s="19">
         <f>truthStateInitialUncertainty!E6</f>
@@ -4606,7 +3746,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>truthStateInitialUncertainty!A7</f>
-        <v>sig_vsz</v>
+        <v>sig_vz</v>
       </c>
       <c r="B7" s="7">
         <f>truthStateInitialUncertainty!B7</f>
@@ -4618,7 +3758,7 @@
       </c>
       <c r="D7" s="7" t="str">
         <f>truthStateInitialUncertainty!D7</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
+        <v>3-sigma initial velocity uncertainty</v>
       </c>
       <c r="E7" s="19">
         <f>truthStateInitialUncertainty!E7</f>
@@ -4630,7 +3770,7 @@
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_thx</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="47">
         <f>truthStateInitialUncertainty!B8</f>
         <v>30</v>
       </c>
@@ -4640,7 +3780,7 @@
       </c>
       <c r="D8" s="7" t="str">
         <f>truthStateInitialUncertainty!D8</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
+        <v>3-sigma initial attitude uncertainty</v>
       </c>
       <c r="E8" s="19">
         <f>truthStateInitialUncertainty!E8</f>
@@ -4652,7 +3792,7 @@
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_thy</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="47">
         <f>truthStateInitialUncertainty!B9</f>
         <v>30</v>
       </c>
@@ -4662,7 +3802,7 @@
       </c>
       <c r="D9" s="7" t="str">
         <f>truthStateInitialUncertainty!D9</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
+        <v>3-sigma initial attitude uncertainty</v>
       </c>
       <c r="E9" s="19">
         <f>truthStateInitialUncertainty!E9</f>
@@ -4674,7 +3814,7 @@
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_thz</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="47">
         <f>truthStateInitialUncertainty!B10</f>
         <v>30</v>
       </c>
@@ -4684,7 +3824,7 @@
       </c>
       <c r="D10" s="7" t="str">
         <f>truthStateInitialUncertainty!D10</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
+        <v>3-sigma initial attitude uncertainty</v>
       </c>
       <c r="E10" s="19">
         <f>truthStateInitialUncertainty!E10</f>
@@ -4694,9 +3834,9 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f>truthStateInitialUncertainty!A11</f>
-        <v>sig_rbx</v>
-      </c>
-      <c r="B11" s="48">
+        <v>sig_accelx</v>
+      </c>
+      <c r="B11" s="47">
         <f>truthStateInitialUncertainty!B11</f>
         <v>5</v>
       </c>
@@ -4706,7 +3846,7 @@
       </c>
       <c r="D11" s="7" t="str">
         <f>truthStateInitialUncertainty!D11</f>
-        <v>3-sigma initial beacon position uncertainty</v>
+        <v>3-sigma initial accelerometer bias uncertainty</v>
       </c>
       <c r="E11" s="19">
         <f>truthStateInitialUncertainty!E11</f>
@@ -4716,9 +3856,9 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f>truthStateInitialUncertainty!A12</f>
-        <v>sig_rby</v>
-      </c>
-      <c r="B12" s="48">
+        <v>sig_accely</v>
+      </c>
+      <c r="B12" s="47">
         <f>truthStateInitialUncertainty!B12</f>
         <v>5</v>
       </c>
@@ -4728,7 +3868,7 @@
       </c>
       <c r="D12" s="7" t="str">
         <f>truthStateInitialUncertainty!D12</f>
-        <v>3-sigma initial beacon position uncertainty</v>
+        <v>3-sigma initial accelerometer bias uncertainty</v>
       </c>
       <c r="E12" s="19">
         <f>truthStateInitialUncertainty!E12</f>
@@ -4738,9 +3878,9 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f>truthStateInitialUncertainty!A13</f>
-        <v>sig_rbz</v>
-      </c>
-      <c r="B13" s="48">
+        <v>sig_accelz</v>
+      </c>
+      <c r="B13" s="47">
         <f>truthStateInitialUncertainty!B13</f>
         <v>10</v>
       </c>
@@ -4750,7 +3890,7 @@
       </c>
       <c r="D13" s="7" t="str">
         <f>truthStateInitialUncertainty!D13</f>
-        <v>3-sigma initial beacon position uncertainty</v>
+        <v>3-sigma initial accelerometer bias uncertainty</v>
       </c>
       <c r="E13" s="19">
         <f>truthStateInitialUncertainty!E13</f>
@@ -4762,9 +3902,9 @@
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="47">
         <f>truthStateInitialUncertainty!B14</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>truthStateInitialUncertainty!C14</f>
@@ -4776,7 +3916,7 @@
       </c>
       <c r="E14" s="19">
         <f>truthStateInitialUncertainty!E14</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -4784,9 +3924,9 @@
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="47">
         <f>truthStateInitialUncertainty!B15</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>truthStateInitialUncertainty!C15</f>
@@ -4798,7 +3938,7 @@
       </c>
       <c r="E15" s="19">
         <f>truthStateInitialUncertainty!E15</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -4806,9 +3946,9 @@
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="47">
         <f>truthStateInitialUncertainty!B16</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>truthStateInitialUncertainty!C16</f>
@@ -4820,15 +3960,15 @@
       </c>
       <c r="E16" s="19">
         <f>truthStateInitialUncertainty!E16</f>
-        <v>1.6160456036984533E-5</v>
+        <v>1.6160456036984532E-6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
         <f>truthStateInitialUncertainty!A17</f>
-        <v>sig_range</v>
-      </c>
-      <c r="B17" s="48">
+        <v>sig_alt</v>
+      </c>
+      <c r="B17" s="47">
         <f>truthStateInitialUncertainty!B17</f>
         <v>31.5</v>
       </c>
@@ -4838,7 +3978,7 @@
       </c>
       <c r="D17" s="7" t="str">
         <f>truthStateInitialUncertainty!D17</f>
-        <v>3-sigma initial range bias uncertainty</v>
+        <v>3-sigma initial altimeter bias uncertainty</v>
       </c>
       <c r="E17" s="19">
         <f>truthStateInitialUncertainty!E17</f>
@@ -4848,9 +3988,9 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
         <f>truthStateInitialUncertainty!A18</f>
-        <v>sig_doppler</v>
-      </c>
-      <c r="B18" s="48">
+        <v>sig_air</v>
+      </c>
+      <c r="B18" s="47">
         <f>truthStateInitialUncertainty!B18</f>
         <v>3</v>
       </c>
@@ -4860,7 +4000,7 @@
       </c>
       <c r="D18" s="7" t="str">
         <f>truthStateInitialUncertainty!D18</f>
-        <v>3-sigma initial dopler bias uncertainty</v>
+        <v>3-sigma initial airspeed bias uncertainty</v>
       </c>
       <c r="E18" s="19">
         <f>truthStateInitialUncertainty!E18</f>
@@ -4868,267 +4008,25 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="str">
+      <c r="A19" s="8" t="str">
         <f>truthStateInitialUncertainty!A19</f>
-        <v>sig_gravx</v>
-      </c>
-      <c r="B19" s="47">
+        <v>sig_wind</v>
+      </c>
+      <c r="B19" s="38">
         <f>truthStateInitialUncertainty!B19</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="7" t="str">
+        <v>5</v>
+      </c>
+      <c r="C19" s="9" t="str">
         <f>truthStateInitialUncertainty!C19</f>
         <v>g</v>
       </c>
-      <c r="D19" s="7" t="str">
+      <c r="D19" s="9" t="str">
         <f>truthStateInitialUncertainty!D19</f>
-        <v>3-sigma initial grav bias uncertainty</v>
-      </c>
-      <c r="E19" s="19">
+        <v>3-sigma initial windspeed uncertainty</v>
+      </c>
+      <c r="E19" s="21">
         <f>truthStateInitialUncertainty!E19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="str">
-        <f>truthStateInitialUncertainty!A20</f>
-        <v>sig_gravy</v>
-      </c>
-      <c r="B20" s="47">
-        <f>truthStateInitialUncertainty!B20</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f>truthStateInitialUncertainty!C20</f>
-        <v>g</v>
-      </c>
-      <c r="D20" s="7" t="str">
-        <f>truthStateInitialUncertainty!D20</f>
-        <v>3-sigma initial grav bias uncertainty</v>
-      </c>
-      <c r="E20" s="19">
-        <f>truthStateInitialUncertainty!E20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="str">
-        <f>truthStateInitialUncertainty!A21</f>
-        <v>sig_gravz</v>
-      </c>
-      <c r="B21" s="47">
-        <f>truthStateInitialUncertainty!B21</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="7" t="str">
-        <f>truthStateInitialUncertainty!C21</f>
-        <v>g</v>
-      </c>
-      <c r="D21" s="7" t="str">
-        <f>truthStateInitialUncertainty!D21</f>
-        <v>3-sigma initial grav bias uncertainty</v>
-      </c>
-      <c r="E21" s="19">
-        <f>truthStateInitialUncertainty!E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="str">
-        <f>truthStateInitialUncertainty!A22</f>
-        <v>sig_thscx</v>
-      </c>
-      <c r="B22" s="48">
-        <f>truthStateInitialUncertainty!B22</f>
-        <v>200</v>
-      </c>
-      <c r="C22" s="7" t="str">
-        <f>truthStateInitialUncertainty!C22</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D22" s="7" t="str">
-        <f>truthStateInitialUncertainty!D22</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E22" s="19">
-        <f>truthStateInitialUncertainty!E22</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="str">
-        <f>truthStateInitialUncertainty!A23</f>
-        <v>sig_thscy</v>
-      </c>
-      <c r="B23" s="48">
-        <f>truthStateInitialUncertainty!B23</f>
-        <v>200</v>
-      </c>
-      <c r="C23" s="7" t="str">
-        <f>truthStateInitialUncertainty!C23</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f>truthStateInitialUncertainty!D23</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E23" s="19">
-        <f>truthStateInitialUncertainty!E23</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="str">
-        <f>truthStateInitialUncertainty!A24</f>
-        <v>sig_thscz</v>
-      </c>
-      <c r="B24" s="48">
-        <f>truthStateInitialUncertainty!B24</f>
-        <v>200</v>
-      </c>
-      <c r="C24" s="7" t="str">
-        <f>truthStateInitialUncertainty!C24</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D24" s="7" t="str">
-        <f>truthStateInitialUncertainty!D24</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E24" s="19">
-        <f>truthStateInitialUncertainty!E24</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="str">
-        <f>truthStateInitialUncertainty!A25</f>
-        <v>sig_thtcx</v>
-      </c>
-      <c r="B25" s="48">
-        <f>truthStateInitialUncertainty!B25</f>
-        <v>200</v>
-      </c>
-      <c r="C25" s="7" t="str">
-        <f>truthStateInitialUncertainty!C25</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D25" s="7" t="str">
-        <f>truthStateInitialUncertainty!D25</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E25" s="19">
-        <f>truthStateInitialUncertainty!E25</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="str">
-        <f>truthStateInitialUncertainty!A26</f>
-        <v>sig_thtcy</v>
-      </c>
-      <c r="B26" s="48">
-        <f>truthStateInitialUncertainty!B26</f>
-        <v>200</v>
-      </c>
-      <c r="C26" s="7" t="str">
-        <f>truthStateInitialUncertainty!C26</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D26" s="7" t="str">
-        <f>truthStateInitialUncertainty!D26</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E26" s="19">
-        <f>truthStateInitialUncertainty!E26</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="str">
-        <f>truthStateInitialUncertainty!A27</f>
-        <v>sig_thtcz</v>
-      </c>
-      <c r="B27" s="48">
-        <f>truthStateInitialUncertainty!B27</f>
-        <v>200</v>
-      </c>
-      <c r="C27" s="7" t="str">
-        <f>truthStateInitialUncertainty!C27</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D27" s="7" t="str">
-        <f>truthStateInitialUncertainty!D27</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E27" s="19">
-        <f>truthStateInitialUncertainty!E27</f>
-        <v>3.2320912073969063E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="str">
-        <f>truthStateInitialUncertainty!A28</f>
-        <v>sig_rfx</v>
-      </c>
-      <c r="B28" s="48">
-        <f>truthStateInitialUncertainty!B28</f>
-        <v>100</v>
-      </c>
-      <c r="C28" s="7" t="str">
-        <f>truthStateInitialUncertainty!C28</f>
-        <v>m</v>
-      </c>
-      <c r="D28" s="7" t="str">
-        <f>truthStateInitialUncertainty!D28</f>
-        <v>3-sigma initial feature position uncertainty</v>
-      </c>
-      <c r="E28" s="19">
-        <f>truthStateInitialUncertainty!E28</f>
-        <v>33.333333333333336</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="str">
-        <f>truthStateInitialUncertainty!A29</f>
-        <v>sig_rfy</v>
-      </c>
-      <c r="B29" s="48">
-        <f>truthStateInitialUncertainty!B29</f>
-        <v>100</v>
-      </c>
-      <c r="C29" s="7" t="str">
-        <f>truthStateInitialUncertainty!C29</f>
-        <v>m</v>
-      </c>
-      <c r="D29" s="7" t="str">
-        <f>truthStateInitialUncertainty!D29</f>
-        <v>3-sigma initial feature position uncertainty</v>
-      </c>
-      <c r="E29" s="19">
-        <f>truthStateInitialUncertainty!E29</f>
-        <v>33.333333333333336</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="str">
-        <f>truthStateInitialUncertainty!A30</f>
-        <v>sig_rfz</v>
-      </c>
-      <c r="B30" s="49">
-        <f>truthStateInitialUncertainty!B30</f>
-        <v>100</v>
-      </c>
-      <c r="C30" s="9" t="str">
-        <f>truthStateInitialUncertainty!C30</f>
-        <v>m</v>
-      </c>
-      <c r="D30" s="9" t="str">
-        <f>truthStateInitialUncertainty!D30</f>
-        <v>3-sigma initial feature position uncertainty</v>
-      </c>
-      <c r="E30" s="21">
-        <f>truthStateInitialUncertainty!E30</f>
-        <v>33.333333333333336</v>
+        <v>16.350000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -5142,7 +4040,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5167,12 +4065,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
       <c r="B2" s="5">
         <v>5</v>
@@ -5181,7 +4079,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="18">
         <f t="shared" ref="E2:E11" si="0">B2</f>
@@ -5190,7 +4088,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7">
         <v>6</v>
@@ -5199,7 +4097,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
@@ -5208,7 +4106,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="B4" s="7">
         <v>7</v>
@@ -5217,7 +4115,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
@@ -5226,7 +4124,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="B5" s="7">
         <v>0.1</v>
@@ -5235,7 +4133,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
@@ -5244,7 +4142,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>165</v>
+        <v>89</v>
       </c>
       <c r="B6" s="7">
         <v>0.2</v>
@@ -5253,7 +4151,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="0"/>
@@ -5262,7 +4160,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="B7" s="7">
         <v>0.3</v>
@@ -5271,7 +4169,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" si="0"/>
@@ -5280,7 +4178,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="12">
         <v>0.01</v>
@@ -5289,7 +4187,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="0"/>
@@ -5298,7 +4196,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="12">
         <v>0.02</v>
@@ -5307,7 +4205,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="19">
         <f t="shared" si="0"/>
@@ -5316,7 +4214,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="12">
         <v>0.03</v>
@@ -5325,7 +4223,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="19">
         <f t="shared" si="0"/>
@@ -5334,16 +4232,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11" s="48">
+        <v>91</v>
+      </c>
+      <c r="B11" s="47">
         <v>0.05</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>172</v>
+        <v>96</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>173</v>
+        <v>97</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
@@ -5352,16 +4250,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="B12" s="12">
         <v>0.2</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="E12" s="19">
         <f>B12</f>
@@ -5370,16 +4268,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="B13" s="12">
         <v>0.3</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="E13" s="19">
         <f>B13</f>
@@ -5388,16 +4286,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>170</v>
+        <v>94</v>
       </c>
       <c r="B14" s="12">
         <v>0.4</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="E14" s="19">
         <f>B14</f>
@@ -5406,7 +4304,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="12">
         <v>1</v>
@@ -5416,7 +4314,7 @@
         <v>deg/hr</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" s="19">
         <f>RADIANS(B15)/hr2sec</f>
@@ -5425,7 +4323,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
@@ -5435,7 +4333,7 @@
         <v>deg/hr</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="19">
         <f>RADIANS(B16)/hr2sec</f>
@@ -5444,7 +4342,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="12">
         <v>3</v>
@@ -5454,7 +4352,7 @@
         <v>deg/hr</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="19">
         <f>RADIANS(B17)/hr2sec</f>
@@ -5463,7 +4361,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>174</v>
+        <v>98</v>
       </c>
       <c r="B18" s="40">
         <v>1</v>
@@ -5472,7 +4370,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="E18" s="41">
         <f>B18</f>
@@ -5481,7 +4379,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="B19" s="40">
         <v>0.5</v>
@@ -5490,7 +4388,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="E19" s="41">
         <f>B19</f>
@@ -5499,16 +4397,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B20" s="40">
         <v>0.5</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
       <c r="E20" s="43">
         <f t="shared" ref="E20:E22" si="1">B20</f>
@@ -5517,16 +4415,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="B21" s="40">
         <v>0.6</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
       <c r="E21" s="43">
         <f t="shared" si="1"/>
@@ -5535,16 +4433,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="B22" s="42">
         <v>0.7</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>182</v>
+        <v>76</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>106</v>
       </c>
       <c r="E22" s="44">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Committing updated config file and adding debugging guide for reference
</commit_message>
<xml_diff>
--- a/simulations/monteCarlo/config.xlsx
+++ b/simulations/monteCarlo/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Repositories\rocket2020\simulations\monteCarlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FBE9A5-999C-4EF5-A72C-10CA3B7FF15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DA75AC-ECFF-40FC-99DF-F4F8910E4236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10350" yWindow="2745" windowWidth="21600" windowHeight="11385" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="2715" windowWidth="21600" windowHeight="11385" tabRatio="894" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="218">
   <si>
     <t>Value</t>
   </si>
@@ -320,9 +320,6 @@
     <t>del_vz</t>
   </si>
   <si>
-    <t>del_m</t>
-  </si>
-  <si>
     <t>del_accelx</t>
   </si>
   <si>
@@ -338,24 +335,12 @@
     <t>kg</t>
   </si>
   <si>
-    <t>Injected mass error</t>
-  </si>
-  <si>
     <t>del_alt</t>
   </si>
   <si>
     <t>del_air</t>
   </si>
   <si>
-    <t>del_wx</t>
-  </si>
-  <si>
-    <t>del_wy</t>
-  </si>
-  <si>
-    <t>del_wz</t>
-  </si>
-  <si>
     <t>Injected accel bias error</t>
   </si>
   <si>
@@ -363,9 +348,6 @@
   </si>
   <si>
     <t>Injected airspeed bias error</t>
-  </si>
-  <si>
-    <t>Injected windspeed error</t>
   </si>
   <si>
     <t>tau_alt</t>
@@ -854,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -897,9 +879,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -907,6 +886,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,7 +1422,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B11" s="15">
         <v>3500</v>
@@ -1460,7 +1440,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B12" s="15">
         <v>3500</v>
@@ -1478,7 +1458,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B13" s="15">
         <v>2000</v>
@@ -1517,7 +1497,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>4</v>
@@ -1527,7 +1507,7 @@
       </c>
       <c r="E15" s="19">
         <f>B15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,21 +1616,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="43">
         <v>399000000000000</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E2" s="19">
         <f t="shared" ref="E2:E5" si="0">B2</f>
@@ -1661,12 +1641,12 @@
       <c r="A3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="44">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="28" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
@@ -1675,16 +1655,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="47">
+        <v>104</v>
+      </c>
+      <c r="B4" s="44">
         <v>6371000</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
@@ -1695,14 +1675,14 @@
       <c r="A5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="44">
         <v>6378137</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
@@ -1711,16 +1691,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="47">
+        <v>105</v>
+      </c>
+      <c r="B6" s="44">
         <v>9.81</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E6" s="19">
         <f>B6</f>
@@ -1765,12 +1745,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B2" s="39">
         <v>41.666200000000003</v>
@@ -1779,7 +1759,7 @@
         <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E2" s="18">
         <f>RADIANS(B2)</f>
@@ -1791,16 +1771,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" s="47">
+        <v>200</v>
+      </c>
+      <c r="B3" s="44">
         <v>-111.4632</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E3" s="18">
         <f>RADIANS(B3)</f>
@@ -1812,7 +1792,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B4" s="12">
         <v>1380</v>
@@ -1821,7 +1801,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E4" s="19">
         <f>B4</f>
@@ -1833,26 +1813,26 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B5" s="47">
+        <v>212</v>
+      </c>
+      <c r="B5" s="44">
         <v>3</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E5" s="19">
         <f>B5</f>
         <v>3</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="44"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B6" s="26">
         <v>90</v>
@@ -1861,7 +1841,7 @@
         <v>67</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E6" s="19">
         <f>RADIANS(B6)</f>
@@ -1873,16 +1853,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="B7" s="50">
+        <v>202</v>
+      </c>
+      <c r="B7" s="47">
         <v>85</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E7" s="21">
         <f>RADIANS(B7)</f>
@@ -1929,22 +1909,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="46">
+        <v>111</v>
+      </c>
+      <c r="B2" s="43">
         <f>PI()*(B4/2)^2</f>
         <v>2.8352873698647883E-2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E2" s="19">
         <f t="shared" ref="E2:E40" si="0">B2</f>
@@ -1953,17 +1933,17 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="46">
+        <v>144</v>
+      </c>
+      <c r="B3" s="43">
         <f>PI()*B4*B5</f>
         <v>1.1341149479459152</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E3" s="19">
         <f>B3</f>
@@ -1972,16 +1952,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="47">
+        <v>112</v>
+      </c>
+      <c r="B4" s="44">
         <v>0.19</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
@@ -1990,16 +1970,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="47">
+        <v>118</v>
+      </c>
+      <c r="B5" s="44">
         <v>1.9</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
@@ -2008,16 +1988,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="47">
+        <v>113</v>
+      </c>
+      <c r="B6" s="44">
         <v>1.98</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="0"/>
@@ -2026,16 +2006,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="47">
+        <v>114</v>
+      </c>
+      <c r="B7" s="44">
         <v>1.66</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" si="0"/>
@@ -2044,16 +2024,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="47">
+        <v>115</v>
+      </c>
+      <c r="B8" s="44">
         <v>1.5</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="0"/>
@@ -2062,9 +2042,9 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="B9" s="47">
+        <v>207</v>
+      </c>
+      <c r="B9" s="44">
         <v>0.2</v>
       </c>
       <c r="C9" s="28"/>
@@ -2076,16 +2056,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" s="40">
         <v>2100</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E10" s="19">
         <f t="shared" si="0"/>
@@ -2094,7 +2074,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B11" s="40">
         <v>199</v>
@@ -2103,7 +2083,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
@@ -2112,16 +2092,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B12" s="40">
         <v>6.1359000000000001E-4</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -2130,7 +2110,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" s="40">
         <v>0.25</v>
@@ -2139,7 +2119,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E13" s="19">
         <f>B13</f>
@@ -2148,17 +2128,17 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="48">
+        <v>137</v>
+      </c>
+      <c r="B14" s="45">
         <f>B13*B15 - 0.5*B15^2*(TAN(E18) + TAN(E19))</f>
         <v>6.7469582591336119E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
@@ -2167,7 +2147,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" s="40">
         <v>0.3</v>
@@ -2176,7 +2156,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="0"/>
@@ -2185,7 +2165,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B16" s="40">
         <v>0.01</v>
@@ -2194,7 +2174,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="0"/>
@@ -2203,14 +2183,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B17" s="2">
         <f>B15^2/B14</f>
         <v>1.3339344419118586</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E17" s="19">
         <f t="shared" si="0"/>
@@ -2219,16 +2199,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B18" s="40">
         <v>9.5</v>
       </c>
       <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>149</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>155</v>
       </c>
       <c r="E18" s="19">
         <f>RADIANS(B18)</f>
@@ -2237,16 +2217,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E19" s="19">
         <f>RADIANS(B19)</f>
@@ -2255,7 +2235,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B20" s="40">
         <f>B4</f>
@@ -2272,7 +2252,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B21" s="40">
         <f>B4</f>
@@ -2289,13 +2269,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B22" s="40">
         <v>4</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E22" s="19">
         <f t="shared" si="0"/>
@@ -2304,13 +2284,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B23" s="40">
         <v>20</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E23" s="19">
         <f t="shared" si="0"/>
@@ -2319,13 +2299,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B24" s="40">
         <v>506</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E24" s="19">
         <f t="shared" si="0"/>
@@ -2334,13 +2314,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B25" s="40">
         <v>506</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E25" s="19">
         <f t="shared" si="0"/>
@@ -2349,13 +2329,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E26" s="19">
         <f t="shared" si="0"/>
@@ -2364,13 +2344,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B27" s="40">
         <v>15</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E27" s="19">
         <f t="shared" si="0"/>
@@ -2379,13 +2359,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B28" s="40">
         <v>0</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E28" s="19">
         <f t="shared" si="0"/>
@@ -2394,7 +2374,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B29" s="40">
         <v>0</v>
@@ -2407,13 +2387,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B30" s="2">
         <v>1E-3</v>
       </c>
       <c r="C30" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E30" s="19">
         <f>1/RADIANS(1/B30)</f>
@@ -2422,13 +2402,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B31" s="2">
         <v>1E-3</v>
       </c>
       <c r="C31" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E31" s="19">
         <f>1/RADIANS(1/B31)</f>
@@ -2437,7 +2417,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B32" s="2">
         <v>2E-3</v>
@@ -2449,7 +2429,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B33" s="2">
         <v>0.3</v>
@@ -2461,7 +2441,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B34" s="2">
         <v>0.4</v>
@@ -2473,13 +2453,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B35" s="2">
         <v>3.835</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E35" s="19">
         <f t="shared" si="0"/>
@@ -2488,13 +2468,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B36" s="2">
         <v>2.4889999999999999</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E36" s="19">
         <f t="shared" si="0"/>
@@ -2503,14 +2483,14 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B37" s="2">
         <f>1.012+0.984+0.0642</f>
         <v>2.0602</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E37" s="19">
         <f t="shared" si="0"/>
@@ -2519,13 +2499,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B38" s="2">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="19">
         <f t="shared" si="0"/>
@@ -2534,13 +2514,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B39" s="2">
         <v>0.2</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E39" s="19">
         <f t="shared" si="0"/>
@@ -2549,14 +2529,14 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B40" s="2">
         <f>SUM(B30:B39)</f>
         <v>9.344199999999999</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40" s="19">
         <f t="shared" si="0"/>
@@ -2565,7 +2545,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
-      <c r="E41" s="51"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="7"/>
     </row>
   </sheetData>
@@ -2605,7 +2585,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>82</v>
@@ -2755,7 +2735,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B8" s="15">
         <v>31.5</v>
@@ -2764,7 +2744,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" ref="E8:E12" si="0">B8/3</f>
@@ -2773,7 +2753,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B9" s="15">
         <v>3</v>
@@ -2782,7 +2762,7 @@
         <v>76</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E9" s="19">
         <f t="shared" si="0"/>
@@ -2791,7 +2771,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B10" s="11">
         <v>5</v>
@@ -2800,17 +2780,17 @@
         <v>76</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E10" s="19">
         <f>B10/3</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I10" s="45"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B11" s="17">
         <f>B8</f>
@@ -2829,7 +2809,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B12" s="20">
         <f>B9</f>
@@ -2885,12 +2865,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B2" s="5">
         <v>500</v>
@@ -2899,7 +2879,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E2" s="18">
         <f t="shared" ref="E2:E13" si="0">B2/3</f>
@@ -2911,7 +2891,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B3" s="7">
         <v>500</v>
@@ -2920,7 +2900,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
@@ -2932,7 +2912,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B4" s="7">
         <v>500</v>
@@ -2941,7 +2921,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E4" s="19">
         <f t="shared" si="0"/>
@@ -2953,7 +2933,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B5" s="7">
         <v>0.2</v>
@@ -2962,7 +2942,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
@@ -2978,7 +2958,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B6" s="7">
         <v>0.2</v>
@@ -2987,7 +2967,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="0"/>
@@ -3003,7 +2983,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B7" s="7">
         <v>0.2</v>
@@ -3012,7 +2992,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E7" s="19">
         <f t="shared" si="0"/>
@@ -3037,7 +3017,7 @@
         <v>81</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E8" s="19">
         <f>RADIANS(B8)/3600/3</f>
@@ -3061,7 +3041,7 @@
         <v>81</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E9" s="19">
         <f>RADIANS(B9)/3600/3</f>
@@ -3085,7 +3065,7 @@
         <v>81</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E10" s="19">
         <f>RADIANS(B10)/3600/3</f>
@@ -3100,7 +3080,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B11" s="12">
         <v>5</v>
@@ -3109,7 +3089,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
@@ -3121,7 +3101,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B12" s="12">
         <v>5</v>
@@ -3130,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -3142,7 +3122,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B13" s="12">
         <v>10</v>
@@ -3151,7 +3131,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="0"/>
@@ -3189,7 +3169,7 @@
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="44">
         <f>truthStateParams!B6</f>
         <v>1</v>
       </c>
@@ -3213,7 +3193,7 @@
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="44">
         <f>truthStateParams!B6</f>
         <v>1</v>
       </c>
@@ -3235,7 +3215,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B17" s="12">
         <f>truthStateParams!B8</f>
@@ -3245,7 +3225,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E17" s="19">
         <f>B17/3</f>
@@ -3258,7 +3238,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B18" s="12">
         <f>truthStateParams!B9</f>
@@ -3268,7 +3248,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E18" s="19">
         <f>B18/3</f>
@@ -3281,18 +3261,18 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B19" s="38">
         <f>truthStateParams!B10</f>
         <v>5</v>
       </c>
-      <c r="C19" s="49" t="str">
+      <c r="C19" s="46" t="str">
         <f>truthStateParams!$C$3</f>
         <v>g</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E19" s="21">
         <f>B19*g2mps2/3</f>
@@ -3342,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3531,7 +3511,7 @@
         <f>truthStateParams!A10</f>
         <v>sig_wind_ss</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="43">
         <f>truthStateParams!B10</f>
         <v>5</v>
       </c>
@@ -3630,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3770,7 +3750,7 @@
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_thx</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="44">
         <f>truthStateInitialUncertainty!B8</f>
         <v>30</v>
       </c>
@@ -3792,7 +3772,7 @@
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_thy</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="44">
         <f>truthStateInitialUncertainty!B9</f>
         <v>30</v>
       </c>
@@ -3814,7 +3794,7 @@
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_thz</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="44">
         <f>truthStateInitialUncertainty!B10</f>
         <v>30</v>
       </c>
@@ -3836,7 +3816,7 @@
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_accelx</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="44">
         <f>truthStateInitialUncertainty!B11</f>
         <v>5</v>
       </c>
@@ -3858,7 +3838,7 @@
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_accely</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="44">
         <f>truthStateInitialUncertainty!B12</f>
         <v>5</v>
       </c>
@@ -3880,7 +3860,7 @@
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_accelz</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="44">
         <f>truthStateInitialUncertainty!B13</f>
         <v>10</v>
       </c>
@@ -3902,7 +3882,7 @@
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="44">
         <f>truthStateInitialUncertainty!B14</f>
         <v>1</v>
       </c>
@@ -3924,7 +3904,7 @@
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="44">
         <f>truthStateInitialUncertainty!B15</f>
         <v>1</v>
       </c>
@@ -3946,7 +3926,7 @@
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="44">
         <f>truthStateInitialUncertainty!B16</f>
         <v>1</v>
       </c>
@@ -3968,7 +3948,7 @@
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_alt</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="44">
         <f>truthStateInitialUncertainty!B17</f>
         <v>31.5</v>
       </c>
@@ -3990,7 +3970,7 @@
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_air</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="44">
         <f>truthStateInitialUncertainty!B18</f>
         <v>3</v>
       </c>
@@ -4037,10 +4017,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4065,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4082,7 +4062,7 @@
         <v>51</v>
       </c>
       <c r="E2" s="18">
-        <f t="shared" ref="E2:E11" si="0">B2</f>
+        <f t="shared" ref="E2:E10" si="0">B2</f>
         <v>5</v>
       </c>
     </row>
@@ -4234,18 +4214,18 @@
       <c r="A11" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="47">
-        <v>0.05</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>97</v>
+      <c r="B11" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="E11" s="19">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <f>B11</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4253,17 +4233,17 @@
         <v>92</v>
       </c>
       <c r="B12" s="12">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E12" s="19">
         <f>B12</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4271,43 +4251,44 @@
         <v>93</v>
       </c>
       <c r="B13" s="12">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E13" s="19">
         <f>B13</f>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B14" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>95</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="11" t="str">
+        <f>truthStateParams!$C$6</f>
+        <v>deg/hr</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="E14" s="19">
-        <f>B14</f>
-        <v>0.4</v>
+        <f>RADIANS(B14)/hr2sec</f>
+        <v>4.8481368110953598E-6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="11" t="str">
         <f>truthStateParams!$C$6</f>
@@ -4318,15 +4299,15 @@
       </c>
       <c r="E15" s="19">
         <f>RADIANS(B15)/hr2sec</f>
-        <v>4.8481368110953598E-6</v>
+        <v>9.6962736221907197E-6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="11" t="str">
         <f>truthStateParams!$C$6</f>
@@ -4337,116 +4318,43 @@
       </c>
       <c r="E16" s="19">
         <f>RADIANS(B16)/hr2sec</f>
-        <v>9.6962736221907197E-6</v>
+        <v>1.454441043328608E-5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="12">
-        <v>3</v>
-      </c>
-      <c r="C17" s="11" t="str">
-        <f>truthStateParams!$C$6</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="19">
-        <f>RADIANS(B17)/hr2sec</f>
-        <v>1.454441043328608E-5</v>
+      <c r="A17" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="40">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="41">
+        <f>B17</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="40">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="49">
         <f>B18</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="40">
         <v>0.5</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="41">
-        <f>B19</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="43">
-        <f t="shared" ref="E20:E22" si="1">B20</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="40">
-        <v>0.6</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="43">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="42">
-        <v>0.7</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="44">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>